<commit_message>
worked on assign 2, started session 6 slides
</commit_message>
<xml_diff>
--- a/assignments/assign2/params_assign2.xlsx
+++ b/assignments/assign2/params_assign2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/assignments/assign2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FA76211-019C-754B-9CB1-AEECF0D65FFF}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5675007-DEAF-9049-90C6-F2E76133EBC9}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-6700" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
+    <workbookView xWindow="-51200" yWindow="-6700" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="daly_params" sheetId="6" r:id="rId1"/>
@@ -728,13 +728,13 @@
     <t>hiv_AIDS_RD</t>
   </si>
   <si>
-    <t>Age_lower</t>
-  </si>
-  <si>
     <t>Male_2016</t>
   </si>
   <si>
     <t>Female_2016</t>
+  </si>
+  <si>
+    <t>age_lower</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -998,7 +998,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -2198,7 +2198,7 @@
   </sheetPr>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -6020,8 +6020,8 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6041,13 +6041,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Updated and released Assignment 2
</commit_message>
<xml_diff>
--- a/assignments/assign2/params_assign2.xlsx
+++ b/assignments/assign2/params_assign2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/assignments/assign2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epib-676/assignments/assign2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B18F506E-019E-1045-B674-3E6E3FEFC8A9}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{2232317A-8042-AC45-A8F0-68118D90C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{164F1F76-4452-8547-A685-5BD071558473}"/>
   <bookViews>
-    <workbookView xWindow="-33380" yWindow="2840" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
+    <workbookView xWindow="-33380" yWindow="2840" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="rewards" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="107">
   <si>
     <t>Age Group</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>HIV subclinical year 2</t>
-  </si>
-  <si>
-    <t>HIV subclinical year 3+</t>
   </si>
   <si>
     <t>AIDS on AVT year 1</t>
@@ -498,14 +495,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -543,7 +536,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -649,7 +642,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -791,7 +784,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -804,16 +797,16 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="2"/>
-    <col min="4" max="4" width="31.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
     <col min="5" max="5" width="17.5" style="2" customWidth="1"/>
     <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
@@ -823,13 +816,13 @@
         <v>21</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>62</v>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>25</v>
@@ -837,16 +830,16 @@
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="6">
+        <v>62</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="6">
         <v>584.55999999999995</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>30</v>
@@ -854,16 +847,16 @@
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="6">
+        <v>63</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="6">
         <v>329.56</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>30</v>
@@ -871,16 +864,16 @@
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="6">
+        <v>59</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="6">
         <v>1150</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>30</v>
@@ -888,279 +881,279 @@
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="6">
+        <v>150</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="6">
-        <v>150</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="6">
+        <v>186.7</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="6">
-        <v>186.7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="6">
+        <v>64.521795064417915</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="6">
-        <v>64.521795064417915</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="6">
+        <v>57.015127896931176</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="6">
-        <v>57.015127896931176</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="6">
+        <v>46.35</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="6">
-        <v>46.35</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="4">
+        <v>69</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="4">
         <v>0</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="4">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="4">
         <v>0</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="4">
+        <v>71</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="4">
         <v>0</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="4">
+        <v>72</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="4">
         <f>0.5*0.274</f>
         <v>0.13700000000000001</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="4">
         <f>0.25*0.274+0.75*0.078</f>
         <v>0.127</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="4">
+        <v>48</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="4">
         <v>7.8E-2</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="4">
+        <v>51</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="4">
         <v>7.8E-2</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="4">
+        <v>53</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="4">
         <v>7.8E-2</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="4">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="4">
         <f>0.5*0.582+0.5*0.078</f>
         <v>0.32999999999999996</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="4">
+        <v>55</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="4">
         <f>0.75*0.078+0.25*0.582</f>
         <v>0.20399999999999999</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="4">
+        <v>59</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="4">
         <f>0.75*0.078+0.25*0.582</f>
         <v>0.20399999999999999</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="E20" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1177,16 +1170,17 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P14" sqref="P14"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="40" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12.6640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="25.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="27" style="2" bestFit="1" customWidth="1"/>
@@ -1195,13 +1189,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>24</v>
@@ -1210,7 +1204,7 @@
         <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>21</v>
@@ -1224,10 +1218,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>43</v>
@@ -1250,10 +1244,10 @@
         <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>33</v>
@@ -1274,10 +1268,10 @@
         <v>45</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>43</v>
@@ -1300,10 +1294,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>35</v>
@@ -1324,10 +1318,10 @@
         <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>38</v>
@@ -1342,7 +1336,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1350,13 +1344,13 @@
         <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>36</v>
@@ -1368,7 +1362,7 @@
         <v>26</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1376,10 +1370,10 @@
         <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>38</v>
@@ -1394,7 +1388,7 @@
         <v>26</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1402,13 +1396,13 @@
         <v>34</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>39</v>
@@ -1420,71 +1414,71 @@
         <v>26</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F11" s="4">
         <v>999</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>36</v>
@@ -1496,7 +1490,7 @@
         <v>26</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1504,13 +1498,13 @@
         <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>39</v>
@@ -1522,7 +1516,7 @@
         <v>26</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1530,13 +1524,13 @@
         <v>41</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>27</v>
@@ -1556,10 +1550,10 @@
         <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>38</v>
@@ -1577,16 +1571,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>27</v>
@@ -1604,13 +1598,13 @@
         <v>42</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>27</v>
@@ -1622,21 +1616,21 @@
         <v>28</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>27</v>
@@ -1648,21 +1642,21 @@
         <v>28</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>27</v>
@@ -1674,21 +1668,21 @@
         <v>28</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>27</v>
@@ -1700,21 +1694,21 @@
         <v>28</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>27</v>
@@ -1731,16 +1725,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>27</v>
@@ -1755,16 +1749,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="C23" s="4" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>27</v>
@@ -1781,16 +1775,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>27</v>
@@ -1807,16 +1801,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>27</v>
@@ -1831,16 +1825,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>27</v>
@@ -1857,16 +1851,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>27</v>
@@ -1943,16 +1937,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>